<commit_message>
Removed old dependencies for Fred and Local vintages + added and tested new ones
</commit_message>
<xml_diff>
--- a/models/US_no_core_rt/data/US_fred.xlsx
+++ b/models/US_no_core_rt/data/US_fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_no_core_rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9348B6A4-951B-1546-B709-3ED2AAD20FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35F4083-5530-5C48-95AA-BE81DE9789AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:AMG6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new draft for get_dataflow
</commit_message>
<xml_diff>
--- a/models/US_no_core_rt/data/US_fred.xlsx
+++ b/models/US_no_core_rt/data/US_fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_no_core_rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35F4083-5530-5C48-95AA-BE81DE9789AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F168D1-505A-E248-B4B8-6972F55B5E92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>frequency</t>
   </si>
@@ -68,13 +68,31 @@
   </si>
   <si>
     <t>unit</t>
+  </si>
+  <si>
+    <t>MNEMONIC</t>
+  </si>
+  <si>
+    <t>URATE</t>
+  </si>
+  <si>
+    <t>EMPL</t>
+  </si>
+  <si>
+    <t>INFL</t>
+  </si>
+  <si>
+    <t>EXP INFL</t>
+  </si>
+  <si>
+    <t>GDP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,6 +107,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,10 +150,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -129,8 +163,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text 2" xfId="1" xr:uid="{5CB3ECAD-2E77-384A-ACD1-8CA865064DF3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,96 +484,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMG6"/>
+  <dimension ref="A1:AMH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1021" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1022" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AMG1"/>
+      <c r="AMH1"/>
     </row>
-    <row r="2" spans="1:1021" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1021" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1021" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1021" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1021" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>